<commit_message>
Divine Order - 3017163907 번역 갱신
</commit_message>
<xml_diff>
--- a/Data/Divine Order - 3017163907/3017163907.xlsx
+++ b/Data/Divine Order - 3017163907/3017163907.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stone\Desktop\Divine Order - 3017163907\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\SteamLibrary\steamapps\common\RimWorld\Mods\MOD KOREAN TRANSLATE\1.4\Botch medieval\Divine Order - 3017163907\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0F1ED8A-473B-48AF-B485-929EC86996F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DC5CC34-2825-4600-940F-A7AD58D71374}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1028" uniqueCount="657">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1085" uniqueCount="693">
   <si>
     <t>Class+Node [(Identifier (Key)]</t>
   </si>
@@ -1985,14 +1985,6 @@
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
-    <t>BotchJob_SacredTablet.comps.0.completedLetterTitle</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>BotchJob_SacredTablet.comps.0.completedLetterText</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
     <t>{PARENT_label} studied: {RESEARCH} unlocked</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
@@ -2023,6 +2015,127 @@
   </si>
   <si>
     <t>ThingDef+BotchJob_DivineOrderRitualCircle.label</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>DamageDef: BotchJob_DivineOrderStaffBlast.label 'divine judgement'</t>
+  </si>
+  <si>
+    <t>DamageDef: BotchJob_DivineOrderStaffBlast.deathMessage '{0} has been incinerated by divine light.'</t>
+  </si>
+  <si>
+    <t>ResearchProjectDef: BotchJob_DivineOrderStaffResearch.label 'staff of divine judgement'</t>
+  </si>
+  <si>
+    <t>ResearchProjectDef: BotchJob_DivineOrderStaffResearch.description 'Learn to craft the staff of divine judgement, the ultimate weapon of the divine order.'</t>
+  </si>
+  <si>
+    <t>ThingDef: BotchJob_DivineJudgementStaff.label 'staff of divine judgement'</t>
+  </si>
+  <si>
+    <t>ThingDef: BotchJob_DivineJudgementStaff.description 'The ultimate weapon of the Divine order. A grand, ornate staff that radiates divine power.\n\nWielding this staff grants the ability to call upon the power of the gods to deliver divine judgement, devastating an area with cleansing light.'</t>
+  </si>
+  <si>
+    <t>ThingDef: BotchJob_DivineJudgementStaff.tools.shaft.label 'shaft'</t>
+  </si>
+  <si>
+    <t>ThingDef: BotchJob_DivineJudgementStaff.verbs.divine_judgement.label 'divine judgement'</t>
+  </si>
+  <si>
+    <t>ThingDef: BotchJob_DivineOrderStaffThrown.label 'divine blast'</t>
+  </si>
+  <si>
+    <t>BotchJob_DivineOrderStaffBlast.label</t>
+  </si>
+  <si>
+    <t>BotchJob_DivineOrderStaffBlast.deathMessage</t>
+  </si>
+  <si>
+    <t>BotchJob_DivineOrderStaffResearch.label</t>
+  </si>
+  <si>
+    <t>BotchJob_DivineOrderStaffResearch.description</t>
+  </si>
+  <si>
+    <t>BotchJob_DivineJudgementStaff.label</t>
+  </si>
+  <si>
+    <t>BotchJob_DivineJudgementStaff.description</t>
+  </si>
+  <si>
+    <t>BotchJob_DivineJudgementStaff.tools.shaft.label</t>
+  </si>
+  <si>
+    <t>BotchJob_DivineJudgementStaff.verbs.divine_judgement.label</t>
+  </si>
+  <si>
+    <t>BotchJob_DivineOrderStaffThrown.label</t>
+  </si>
+  <si>
+    <t>divine judgement</t>
+  </si>
+  <si>
+    <t>{0} has been incinerated by divine light.</t>
+  </si>
+  <si>
+    <t>staff of divine judgement</t>
+  </si>
+  <si>
+    <t>Learn to craft the staff of divine judgement, the ultimate weapon of the divine order.</t>
+  </si>
+  <si>
+    <t>The ultimate weapon of the Divine order. A grand, ornate staff that radiates divine power.\n\nWielding this staff grants the ability to call upon the power of the gods to deliver divine judgement, devastating an area with cleansing light.</t>
+  </si>
+  <si>
+    <t>divine blast</t>
+  </si>
+  <si>
+    <t>디바인 저지먼트</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>{0}(은)는 신성한 빛에 의해 소각되었습니다.</t>
+  </si>
+  <si>
+    <t>디바인 저지먼트 스태프</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>디바인 오더의 궁극의 무기인 디바인 저지먼트 스태프를 연구합니다</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>다바인 오더의 궁극의 무기. 신성한 힘을 발산하는 웅장하고 화려한 지팡이입니다.\n\n이 지팡이를 휘두르면 신들의 힘을 불러내 신성한 심판을 내리고 정화의 빛으로 지역을 파괴할 수 있습니다.</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>스태프</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>디바인 블라스트</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>BotchJob_DivineOrderPlayerFaction.leaderTitle</t>
+  </si>
+  <si>
+    <t>leader</t>
+  </si>
+  <si>
+    <t>BotchJob_DivineOrderStart.label</t>
+  </si>
+  <si>
+    <t>BotchJob_DivineOrderStart.description</t>
+  </si>
+  <si>
+    <t>BotchJob_SacredTablet.comps.CompStudiable.completedLetterText</t>
+  </si>
+  <si>
+    <t>BotchJob_SacredTablet.comps.CompStudiable.completedLetterTitle</t>
+  </si>
+  <si>
+    <t>지도자</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
 </sst>
@@ -2448,24 +2561,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G168"/>
+  <dimension ref="A1:H180"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView tabSelected="1" topLeftCell="A154" workbookViewId="0">
+      <selection activeCell="A177" sqref="A177:A180"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="68.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="56.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="68.375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="56.375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="47.5" customWidth="1"/>
     <col min="5" max="5" width="40.75" customWidth="1"/>
-    <col min="6" max="6" width="24.9140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="41.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2488,7 +2601,7 @@
         <v>635</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="str">
         <f>_xlfn.TEXTJOIN("+",,B2,C2)</f>
         <v>ThingDef+BotchJob_DivineOrderHorse.label</v>
@@ -2513,7 +2626,7 @@
         <v>개량된 말</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="str">
         <f t="shared" ref="A3:A68" si="0">_xlfn.TEXTJOIN("+",,B3,C3)</f>
         <v>ThingDef+BotchJob_DivineOrderHorse.description</v>
@@ -2538,7 +2651,7 @@
         <v>디바인 오더의 말입니다. 일반 말보다 크고 강하며 더 빠릅니다.\n\n상단에 데려가면 상단의 속도를 높일 수 있습니다.</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="str">
         <f t="shared" si="0"/>
         <v>ThingDef+BotchJob_DivineOrderHorse.race.meatLabel</v>
@@ -2563,7 +2676,7 @@
         <v>말 고기</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="str">
         <f t="shared" si="0"/>
         <v>ThingDef+BotchJob_DivineOrderHorse.tools.0.label</v>
@@ -2588,7 +2701,7 @@
         <v>머리</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="str">
         <f t="shared" si="0"/>
         <v>ThingDef+BotchJob_DivineOrderHorse.tools.1.label</v>
@@ -2610,7 +2723,7 @@
         <v>왼쪽 발굽</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="str">
         <f t="shared" si="0"/>
         <v>ThingDef+BotchJob_DivineOrderHorse.tools.2.label</v>
@@ -2632,7 +2745,7 @@
         <v>오른쪽 발굽</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="str">
         <f t="shared" si="0"/>
         <v>ThingDef+BotchJob_DivineOrderCloak.label</v>
@@ -2654,7 +2767,7 @@
         <v>디바인 오더 망토</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="str">
         <f t="shared" si="0"/>
         <v>ThingDef+BotchJob_DivineOrderCloak.description</v>
@@ -2676,7 +2789,7 @@
         <v>천이나 가죽으로 만든 두꺼운 망토입니다.\n\n보통 다른 옷 위에 입으며, 약간의 신체 보호와 함께 비바람을 막아주는 역할을 합니다.</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="str">
         <f t="shared" si="0"/>
         <v>ThingDef+BotchJob_DivineOrderFurCloak.label</v>
@@ -2698,7 +2811,7 @@
         <v>디바인 오더 털 망토</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="str">
         <f t="shared" si="0"/>
         <v>ThingDef+BotchJob_DivineOrderFurCloak.description</v>
@@ -2720,7 +2833,7 @@
         <v>긴 모피 망토. 약간의 신체 보호 기능을 제공하며 추위를 매우 잘 막아줍니다.</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="str">
         <f t="shared" si="0"/>
         <v>ThingDef+BotchJob_DivineOrderZealotRobes.label</v>
@@ -2742,7 +2855,7 @@
         <v>디바인 오더 광신도 로브</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="str">
         <f t="shared" si="0"/>
         <v>ThingDef+BotchJob_DivineOrderZealotRobes.description</v>
@@ -2764,7 +2877,7 @@
         <v>디바인 오더의 광신도들이 착용하는 금빛 장식의 로브입니다. 소량의 신체 보호 효과를 제공하며, 단열 효과가 뛰어나고 착용자의 시전 능력을 약간 향상시킵니다.</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="str">
         <f t="shared" si="0"/>
         <v>ThingDef+BotchJob_DivineOrderHood.label</v>
@@ -2786,7 +2899,7 @@
         <v>디바인 오더 후드</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="str">
         <f t="shared" si="0"/>
         <v>ThingDef+BotchJob_DivineOrderHood.description</v>
@@ -2808,7 +2921,7 @@
         <v>천이다 가죽으로 만든 두꺼운 후드입니다.\n\n약간의 신체적 보호와 함께 비바람을 막아주는 역할을 합니다.</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="str">
         <f t="shared" si="0"/>
         <v>ThingDef+BotchJob_DivineOrderFurHood.label</v>
@@ -2830,7 +2943,7 @@
         <v>디바인 오더 모피 후드</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="str">
         <f t="shared" si="0"/>
         <v>ThingDef+BotchJob_DivineOrderFurHood.description</v>
@@ -2852,7 +2965,7 @@
         <v>두꺼운 모피 안감 후드.\n\n약간의 신체 보호 기능을 제공하며 추위를 매우 잘 차단합니다.</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="str">
         <f t="shared" si="0"/>
         <v>ThingDef+BotchJob_DivineOrderMerchantHat.label</v>
@@ -2874,7 +2987,7 @@
         <v>디바인 오더 상인의 모자</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="str">
         <f t="shared" si="0"/>
         <v>ThingDef+BotchJob_DivineOrderMerchantHat.description</v>
@@ -2896,7 +3009,7 @@
         <v>보석으로 장식된 화려한 모자로, 디바인 오더의 상인들 좋아하는 모자입니다.\n\n거래 시 보너스 효과를 줍니다.</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="str">
         <f t="shared" si="0"/>
         <v>ThingDef+BotchJob_DivineOrderTunic.label</v>
@@ -2918,7 +3031,7 @@
         <v>디바인 오더 튜닉</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="str">
         <f t="shared" si="0"/>
         <v>ThingDef+BotchJob_DivineOrderTunic.description</v>
@@ -2940,7 +3053,7 @@
         <v>천이나 가죽으로 만든 두꺼운 패딩 튜닉입니다.\n\n단독으로 입거나 갑옷 안에 입을 수 있으며 보온성이 뛰어납니다.</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="str">
         <f t="shared" si="0"/>
         <v>ThingDef+BotchJob_DivineOrderBreeches.label</v>
@@ -2962,7 +3075,7 @@
         <v>디바인 오더 바지</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="str">
         <f t="shared" si="0"/>
         <v>ThingDef+BotchJob_DivineOrderBreeches.description</v>
@@ -2984,7 +3097,7 @@
         <v>천이나 가죽으로 만든 일반적인 바지 한 벌입니다.</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="str">
         <f t="shared" si="0"/>
         <v>ThingDef+BotchJob_DivineOrderPlateHelmet.label</v>
@@ -3006,7 +3119,7 @@
         <v>디바인 오더 판금 투구</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="str">
         <f t="shared" si="0"/>
         <v>ThingDef+BotchJob_DivineOrderPlateHelmet.description</v>
@@ -3028,7 +3141,7 @@
         <v>디바인 오더의 스타일로 제작된 튼튼하고 잘 만들어진 판금 투구입니다.\n\n날카로운 공격에 대한 보호력은 뛰어나지만 둔기에는 효과적이지 않으며 착용자의 시야를 제한합니다.</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="str">
         <f t="shared" si="0"/>
         <v>ThingDef+BotchJob_DivineOrderLightHelmet.label</v>
@@ -3050,7 +3163,7 @@
         <v>디바인 오더 가벼운 투구</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="str">
         <f t="shared" si="0"/>
         <v>ThingDef+BotchJob_DivineOrderLightHelmet.description</v>
@@ -3072,7 +3185,7 @@
         <v>디바인 오더의 스타일로 제작된 가벼운 판금 투구입니다.\n\n판금 투구 만큼 보호력이 뛰어나지 않고 머리 아래쪽이 노출되지만, 제작에 필요한 자원이 적고 시야를 제한하지 않습니다.</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="str">
         <f t="shared" si="0"/>
         <v>ThingDef+BotchJob_DivineOrderOpenHelmet.label</v>
@@ -3094,7 +3207,7 @@
         <v>디바인 오더 개방형 투구</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="str">
         <f t="shared" si="0"/>
         <v>ThingDef+BotchJob_DivineOrderOpenHelmet.description</v>
@@ -3116,7 +3229,7 @@
         <v>디바인 오더의 스타일로 제작된 개방형 판금 투구입니다.\n\n넉넉한 보호력을 제공하며 시야를 제한하지 않지만 아랫면이 노출됩니다.</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="str">
         <f t="shared" si="0"/>
         <v>ThingDef+BotchJob_DivineOrderPlateArmor.label</v>
@@ -3138,7 +3251,7 @@
         <v>디바인 오더 판금 갑옷</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="str">
         <f t="shared" si="0"/>
         <v>ThingDef+BotchJob_DivineOrderPlateArmor.description</v>
@@ -3160,7 +3273,7 @@
         <v>디바인 오더의 스타일로 제작된 판금 갑옷 풀세트입니다.\n\n전신을 덮어 상당한 수준의 보호와 추위로부터의 단열 효과를 제공하지만, 착용자의 속도를 느리게 합니다.</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="str">
         <f t="shared" si="0"/>
         <v>ThingDef+BotchJob_DivineOrderBreastplate.label</v>
@@ -3182,7 +3295,7 @@
         <v>디바인 오더 흉갑</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="str">
         <f t="shared" si="0"/>
         <v>ThingDef+BotchJob_DivineOrderBreastplate.description</v>
@@ -3204,7 +3317,7 @@
         <v>망토와 유사한 의복 아래에 착용할 수 있는 견고한 금속 흉갑입니다.\n\n하지만 몸통만 보호하고 착용자의 속도를 약간 느리게 합니다.</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="str">
         <f t="shared" si="0"/>
         <v>ThingDef+BotchJob_DivineOrderCowledHelmet.label</v>
@@ -3226,7 +3339,7 @@
         <v>디바인 오더 카울드 투구</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="str">
         <f t="shared" si="0"/>
         <v>ThingDef+BotchJob_DivineOrderCowledHelmet.description</v>
@@ -3248,7 +3361,7 @@
         <v>가벼운 투구를 덮은 두꺼운 가죽 고깔입니다.\n\n머리의 움직임이나 시야를 방해하지 않으면서도 적당한 수준의 보호와 단열 효과를 제공합니다.</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="str">
         <f t="shared" si="0"/>
         <v>ThingDef+BotchJob_DivineOrderSkirmisherArmor.label</v>
@@ -3270,7 +3383,7 @@
         <v>척후병의 갑옷</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="str">
         <f t="shared" si="0"/>
         <v>ThingDef+BotchJob_DivineOrderSkirmisherArmor.description</v>
@@ -3292,7 +3405,7 @@
         <v>가벼운 흉갑을 덮은 두꺼운 가죽 갑옷입니다.\n\n가벼우면서도 적당한 보호 기능을 제공하며, 추위와 열을 충분히 차단합니다.</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="str">
         <f t="shared" si="0"/>
         <v>ThingDef+BotchJob_CrusaderHelmet.label</v>
@@ -3314,7 +3427,7 @@
         <v>크루세이더 투구</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="str">
         <f t="shared" si="0"/>
         <v>ThingDef+BotchJob_CrusaderHelmet.description</v>
@@ -3336,7 +3449,7 @@
         <v>고귀한 자들의 흔적에서 살아남아 디바인 오더의 크루세이더가 되는 자에게만 수여되는 룬 직물로 장식된 정교한 판금 투구입니다.\n\n성스러운 석판의 힘으로 축복을 받은 이 투구는 착용자의 근접 숙련도를 향상시킵니다.</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="str">
         <f t="shared" si="0"/>
         <v>ThingDef+BotchJob_CrusaderArmor.label</v>
@@ -3358,7 +3471,7 @@
         <v>크루세이더 갑옷</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="str">
         <f t="shared" si="0"/>
         <v>ThingDef+BotchJob_CrusaderArmor.description</v>
@@ -3380,7 +3493,7 @@
         <v>고귀한 자들의 흔적에서 살아남아 디바인 오더의 크루세이더가 되는 자에게만 수여되는 룬 직물로 장식된 정교한 판금 갑옷입니다.\n\n성스러운 석판의 힘으로 축복을 받은 이 갑옷은 착용자의 근접 숙련도를 향상시킵니다.</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="str">
         <f t="shared" si="0"/>
         <v>ThingDef+BotchJob_InquisitorHat.label</v>
@@ -3402,7 +3515,7 @@
         <v>인퀴지터 모자</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="str">
         <f t="shared" si="0"/>
         <v>ThingDef+BotchJob_InquisitorHat.description</v>
@@ -3424,7 +3537,7 @@
         <v>고귀한 자들의 흔적에서 살아남아 디바인 오더의 인퀴지터가 된 자에게만 수여되는 금으로 장식된 정교한 가죽 모자입니다.\n\n성스러운 석판의 힘으로 축복을 받은 이 모자는 착용자의 사격 숙련도를 향상시킵니다.</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="str">
         <f t="shared" si="0"/>
         <v>ThingDef+BotchJob_InquisitorArmor.label</v>
@@ -3446,7 +3559,7 @@
         <v>인퀴지터 복장</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="str">
         <f t="shared" si="0"/>
         <v>ThingDef+BotchJob_InquisitorArmor.description</v>
@@ -3468,7 +3581,7 @@
         <v>고귀한 자들의 흔적에서 살아남아 디바인 오더의 인퀴지터가 된 자에게만 수여되는 금으로 장식된 정교한 가죽 갑옷입니다.\n\n성스러운 석판의 힘으로 축복을 받은 이 갑옷은 착용자의 사격 숙련도를 향상시킵니다.</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="str">
         <f t="shared" si="0"/>
         <v>ThingDef+BotchJob_InquisitorCloak.label</v>
@@ -3490,7 +3603,7 @@
         <v>인퀴지터 망토</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="str">
         <f t="shared" si="0"/>
         <v>ThingDef+BotchJob_InquisitorCloak.description</v>
@@ -3512,7 +3625,7 @@
         <v>디바인 오더의 인퀴지터가 주로 착용하는 금 장식 망토입니다.</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="str">
         <f t="shared" si="0"/>
         <v>ThingDef+BotchJob_HeraldHelmet.label</v>
@@ -3534,7 +3647,7 @@
         <v>헤럴드 투구</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="str">
         <f t="shared" si="0"/>
         <v>ThingDef+BotchJob_HeraldHelmet.description</v>
@@ -3556,7 +3669,7 @@
         <v>고귀한 자들의 흔적에서 살아남아 디바인 오더의 헤럴드가 되는 자에게만 수여되는 룬 직물로 장식된 화려한 판금 투구입니다.\n\n성스러운 석판의 힘으로 축복을 받은 이 투구는 착용자의 시전 숙련도를 향상시킵니다.</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="str">
         <f t="shared" si="0"/>
         <v>ThingDef+BotchJob_HeraldRobes.label</v>
@@ -3578,7 +3691,7 @@
         <v>헤럴드 로브</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="str">
         <f t="shared" si="0"/>
         <v>ThingDef+BotchJob_HeraldRobes.description</v>
@@ -3600,7 +3713,7 @@
         <v>고귀한 자들의 흔적에서 살아남아 디바인 오더의 헤럴드가 되는 자에게만 수여되는 무거운 예복으로 덮인 튼튼한 갑옷입니다.\n\n성스러운 석판의 힘으로 축복을 받은 이 로브는 착용자의 시전 숙련도를 향상시킵니다.</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A52" s="1" t="str">
         <f t="shared" si="0"/>
         <v>ThingDef+BotchJob_DivineOrderShield.label</v>
@@ -3622,7 +3735,7 @@
         <v>디바인 오더 방패</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A53" s="1" t="str">
         <f t="shared" si="0"/>
         <v>ThingDef+BotchJob_DivineOrderShield.description</v>
@@ -3644,7 +3757,7 @@
         <v>디바인 오더의 휘장이 새겨진 견고한 강화된 방패입니다.</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A54" s="1" t="str">
         <f t="shared" si="0"/>
         <v>ThingDef+BotchJob_DivineOrderShield.tools.0.label</v>
@@ -3666,7 +3779,7 @@
         <v>베이스</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A55" s="1" t="str">
         <f t="shared" si="0"/>
         <v>ThingDef+BotchJob_DivineOrderShield.tools.1.label</v>
@@ -3688,7 +3801,7 @@
         <v>중심</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A56" s="1" t="str">
         <f t="shared" si="0"/>
         <v>ThingDef+BotchJob_DivineOrderBanner.label</v>
@@ -3710,7 +3823,7 @@
         <v>디바인 오더 깃발</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A57" s="1" t="str">
         <f t="shared" si="0"/>
         <v>ThingDef+BotchJob_DivineOrderBanner.description</v>
@@ -3732,7 +3845,7 @@
         <v>디바인 오더의 휘장을 나타내는 깃발입니다.</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A58" s="1" t="str">
         <f t="shared" si="0"/>
         <v>ThingDef+BotchJob_SacredTabletPedestal.label</v>
@@ -3754,7 +3867,7 @@
         <v>성스러운 석판 받침대</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A59" s="1" t="str">
         <f t="shared" si="0"/>
         <v>ThingDef+BotchJob_SacredTabletPedestal.description</v>
@@ -3776,7 +3889,7 @@
         <v>성스러운 석판을 전시하는 장식용 받침대입니다.</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A60" s="1" t="str">
         <f t="shared" si="0"/>
         <v>ThingDef+BotchJob_SacredTablet.label</v>
@@ -3798,7 +3911,7 @@
         <v>성스러운 석판</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A61" s="1" t="str">
         <f t="shared" si="0"/>
         <v>ThingDef+BotchJob_SacredTablet.description</v>
@@ -3820,51 +3933,51 @@
         <v>디바인 오더에서 숭배하는 신성한 석판입니다. 신의 축복을 받았다고 믿으며 강력한 장비를 제작하는 데 사용됩니다.</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A62" s="1" t="str">
         <f t="shared" ref="A62:A63" si="1">_xlfn.TEXTJOIN("+",,B62,C62)</f>
-        <v>ThingDef+BotchJob_SacredTablet.comps.0.completedLetterTitle</v>
+        <v>ThingDef+BotchJob_SacredTablet.comps.CompStudiable.completedLetterTitle</v>
       </c>
       <c r="B62" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C62" s="1" t="s">
+        <v>691</v>
+      </c>
+      <c r="D62" s="1" t="s">
         <v>646</v>
-      </c>
-      <c r="D62" s="1" t="s">
-        <v>648</v>
       </c>
       <c r="E62" s="1" t="s">
         <v>588</v>
       </c>
       <c r="G62" t="str">
         <f>IFERROR(VLOOKUP(A62,Update!$C$2:$D$173,2,FALSE),"")</f>
-        <v>{PARENT_label}(을)를 연구해서 {STUDIER_labelShort}(은)는 {RESEARCH} 연구에 대한 영감을 얻었습니다.\n\n이제 학자들이 연구를 시작할 수 있습니다.</v>
-      </c>
-    </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.45">
+        <v/>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A63" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>ThingDef+BotchJob_SacredTablet.comps.0.completedLetterText</v>
+        <v>ThingDef+BotchJob_SacredTablet.comps.CompStudiable.completedLetterText</v>
       </c>
       <c r="B63" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C63" s="1" t="s">
+        <v>690</v>
+      </c>
+      <c r="D63" s="1" t="s">
         <v>647</v>
-      </c>
-      <c r="D63" s="1" t="s">
-        <v>649</v>
       </c>
       <c r="E63" s="1" t="s">
         <v>590</v>
       </c>
       <c r="G63" t="str">
         <f>IFERROR(VLOOKUP(A63,Update!$C$2:$D$173,2,FALSE),"")</f>
-        <v>{PARENT_label} 연구됨 : {RESEARCH} 연구 해제</v>
-      </c>
-    </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.45">
+        <v/>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A64" s="1" t="str">
         <f t="shared" si="0"/>
         <v>ThingDef+BotchJob_DivineOrderMace.label</v>
@@ -3886,7 +3999,7 @@
         <v>디바인 오더 메이스</v>
       </c>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A65" s="1" t="str">
         <f t="shared" si="0"/>
         <v>ThingDef+BotchJob_DivineOrderMace.description</v>
@@ -3908,7 +4021,7 @@
         <v>디바인 오더 스타일로 제작된 단단한 철퇴로, 갑옷을 입은 적에게 둔기 피해를 입힐 수 있습니다.</v>
       </c>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A66" s="1" t="str">
         <f t="shared" si="0"/>
         <v>ThingDef+BotchJob_DivineOrderMace.tools.0.label</v>
@@ -3930,7 +4043,7 @@
         <v>자루</v>
       </c>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A67" s="1" t="str">
         <f t="shared" si="0"/>
         <v>ThingDef+BotchJob_DivineOrderMace.tools.1.label</v>
@@ -3952,7 +4065,7 @@
         <v>머리</v>
       </c>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A68" s="1" t="str">
         <f t="shared" si="0"/>
         <v>ThingDef+BotchJob_DivineOrderShortsword.label</v>
@@ -3974,7 +4087,7 @@
         <v>디바인 오더 숏소드</v>
       </c>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A69" s="1" t="str">
         <f t="shared" ref="A69:A135" si="2">_xlfn.TEXTJOIN("+",,B69,C69)</f>
         <v>ThingDef+BotchJob_DivineOrderShortsword.description</v>
@@ -3996,7 +4109,7 @@
         <v>디바인 오더 스타일로 제작된 숏소드입니다. 가볍고 다루기 쉬워 귀족과 평민 모두에게 이상적인 무기입니다.</v>
       </c>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A70" s="1" t="str">
         <f t="shared" si="2"/>
         <v>ThingDef+BotchJob_DivineOrderShortsword.tools.0.label</v>
@@ -4018,7 +4131,7 @@
         <v>자루</v>
       </c>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A71" s="1" t="str">
         <f t="shared" si="2"/>
         <v>ThingDef+BotchJob_DivineOrderShortsword.tools.1.label</v>
@@ -4040,7 +4153,7 @@
         <v>칼끝</v>
       </c>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A72" s="1" t="str">
         <f t="shared" si="2"/>
         <v>ThingDef+BotchJob_DivineOrderShortsword.tools.2.label</v>
@@ -4062,7 +4175,7 @@
         <v>칼날</v>
       </c>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A73" s="1" t="str">
         <f t="shared" si="2"/>
         <v>ThingDef+BotchJob_DivineOrderLongsword.label</v>
@@ -4084,7 +4197,7 @@
         <v>디바인 오더 롱소드</v>
       </c>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="74" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A74" s="1" t="str">
         <f t="shared" si="2"/>
         <v>ThingDef+BotchJob_DivineOrderLongsword.description</v>
@@ -4106,7 +4219,7 @@
         <v>디바인 오더 스타일로 제작된 멋진 롱소드입니다. 베거나 찌를 수 있는 균형 잡힌 무기입니다.</v>
       </c>
     </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="75" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A75" s="1" t="str">
         <f t="shared" si="2"/>
         <v>ThingDef+BotchJob_DivineOrderLongsword.tools.0.label</v>
@@ -4128,7 +4241,7 @@
         <v>자루</v>
       </c>
     </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="76" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A76" s="1" t="str">
         <f t="shared" si="2"/>
         <v>ThingDef+BotchJob_DivineOrderLongsword.tools.1.label</v>
@@ -4150,7 +4263,7 @@
         <v>칼끝</v>
       </c>
     </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="77" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A77" s="1" t="str">
         <f t="shared" si="2"/>
         <v>ThingDef+BotchJob_DivineOrderLongsword.tools.2.label</v>
@@ -4172,7 +4285,7 @@
         <v>칼날</v>
       </c>
     </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="78" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A78" s="1" t="str">
         <f t="shared" si="2"/>
         <v>ThingDef+BotchJob_DivineOrderBattleStandard.label</v>
@@ -4194,7 +4307,7 @@
         <v>디바인 오더 전쟁기</v>
       </c>
     </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="79" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A79" s="1" t="str">
         <f t="shared" si="2"/>
         <v>ThingDef+BotchJob_DivineOrderBattleStandard.description</v>
@@ -4216,7 +4329,7 @@
         <v>디바인 오더의 깃발이 달린 긴 창입니다. 보통 전투에서 기수가 높이 들고 있지만, 원거리에서 치명적인 공격을 가할 수 있는 효과적인 근접 무기이기도 합니다.</v>
       </c>
     </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="80" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A80" s="1" t="str">
         <f t="shared" si="2"/>
         <v>ThingDef+BotchJob_DivineOrderBattleStandard.tools.0.label</v>
@@ -4238,7 +4351,7 @@
         <v>창 대</v>
       </c>
     </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="81" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A81" s="1" t="str">
         <f t="shared" si="2"/>
         <v>ThingDef+BotchJob_DivineOrderBattleStandard.tools.1.label</v>
@@ -4260,7 +4373,7 @@
         <v>창끝</v>
       </c>
     </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="82" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A82" s="1" t="str">
         <f t="shared" si="2"/>
         <v>ThingDef+BotchJob_DivineOrderWarhammer.label</v>
@@ -4282,7 +4395,7 @@
         <v>디바인 오더 워해머</v>
       </c>
     </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="83" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A83" s="1" t="str">
         <f t="shared" si="2"/>
         <v>ThingDef+BotchJob_DivineOrderWarhammer.description</v>
@@ -4304,7 +4417,7 @@
         <v>디바인 오더 스타일로 제작된 양손 대형 워해머입니다. 갑옷을 입은 적에게 매우 효과적인 둔탁한 일격을 가할 수 있습니다.</v>
       </c>
     </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="84" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A84" s="1" t="str">
         <f t="shared" si="2"/>
         <v>ThingDef+BotchJob_DivineOrderWarhammer.tools.0.label</v>
@@ -4326,7 +4439,7 @@
         <v>손잡이</v>
       </c>
     </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="85" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A85" s="1" t="str">
         <f t="shared" si="2"/>
         <v>ThingDef+BotchJob_DivineOrderWarhammer.tools.1.label</v>
@@ -4348,7 +4461,7 @@
         <v>머리</v>
       </c>
     </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="86" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A86" s="1" t="str">
         <f t="shared" si="2"/>
         <v>ThingDef+BotchJob_DivineOrderGreatsword.label</v>
@@ -4370,7 +4483,7 @@
         <v>디바인 오더 그레이트소드</v>
       </c>
     </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="87" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A87" s="1" t="str">
         <f t="shared" si="2"/>
         <v>ThingDef+BotchJob_DivineOrderGreatsword.description</v>
@@ -4392,7 +4505,7 @@
         <v>디바인 오더 스타일로 제작된 커다란 그레이트소드입니다. 휘두르는 속도는 느리지만 숙련자의 손에 쥐어지면 치명적인 베기 공격을 가할 수 있습니다.</v>
       </c>
     </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="88" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A88" s="1" t="str">
         <f t="shared" si="2"/>
         <v>ThingDef+BotchJob_DivineOrderGreatsword.tools.0.label</v>
@@ -4414,7 +4527,7 @@
         <v>자루</v>
       </c>
     </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="89" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A89" s="1" t="str">
         <f t="shared" si="2"/>
         <v>ThingDef+BotchJob_DivineOrderGreatsword.tools.1.label</v>
@@ -4436,7 +4549,7 @@
         <v>칼날</v>
       </c>
     </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="90" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A90" s="1" t="str">
         <f t="shared" si="2"/>
         <v>ThingDef+BotchJob_DivineOrderPistol.label</v>
@@ -4458,7 +4571,7 @@
         <v>디바인 오더 피스톨</v>
       </c>
     </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="91" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A91" s="1" t="str">
         <f t="shared" ref="A91" si="3">_xlfn.TEXTJOIN("+",,B91,C91)</f>
         <v>ThingDef+BotchJob_DivineOrderPistol.verbs.Verb_Shoot.label</v>
@@ -4478,7 +4591,7 @@
         <v>디바인 오더 피스톨</v>
       </c>
     </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="92" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A92" s="1" t="str">
         <f t="shared" si="2"/>
         <v>ThingDef+BotchJob_DivineOrderPistol.description</v>
@@ -4500,7 +4613,7 @@
         <v>부싯돌 발사 장치가 달린 화려한 피스톨입니다. 대부분의 일반 갑옷을 뚫을 수 있는 강력한 탄환을 발사하지만 재장전 속도가 느립니다.</v>
       </c>
     </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="93" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A93" s="1" t="str">
         <f t="shared" si="2"/>
         <v>ThingDef+BotchJob_DivineOrderPistol.tools.0.label</v>
@@ -4522,7 +4635,7 @@
         <v>손잡이</v>
       </c>
     </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="94" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A94" s="1" t="str">
         <f t="shared" si="2"/>
         <v>ThingDef+BotchJob_DivineOrderPistol.tools.1.label</v>
@@ -4544,7 +4657,7 @@
         <v>총열</v>
       </c>
     </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="95" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A95" s="1" t="str">
         <f t="shared" si="2"/>
         <v>ThingDef+BotchJob_DivineOrderPistolBullet.label</v>
@@ -4566,7 +4679,7 @@
         <v>피스톨 총알</v>
       </c>
     </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="96" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A96" s="1" t="str">
         <f t="shared" si="2"/>
         <v>ThingDef+BotchJob_DivineOrderCrossbow.label</v>
@@ -4588,7 +4701,7 @@
         <v>디바인 오더 석궁</v>
       </c>
     </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="97" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A97" s="1" t="str">
         <f t="shared" ref="A97" si="4">_xlfn.TEXTJOIN("+",,B97,C97)</f>
         <v>ThingDef+BotchJob_DivineOrderCrossbow.verbs.Verb_Shoot.label</v>
@@ -4608,7 +4721,7 @@
         <v>디바인 오더 석궁</v>
       </c>
     </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="98" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A98" s="1" t="str">
         <f t="shared" si="2"/>
         <v>ThingDef+BotchJob_DivineOrderCrossbow.description</v>
@@ -4630,7 +4743,7 @@
         <v>디바인 오더 스타일로 제작된 석궁입니다. 활보다 사용하기 쉽고 갑옷을 뚫을 수 있지만 재장전 속도가 느립니다.</v>
       </c>
     </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="99" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A99" s="1" t="str">
         <f t="shared" si="2"/>
         <v>ThingDef+BotchJob_DivineOrderCrossbow.tools.0.label</v>
@@ -4652,7 +4765,7 @@
         <v>활대</v>
       </c>
     </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="100" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A100" s="1" t="str">
         <f t="shared" si="2"/>
         <v>ThingDef+BotchJob_DivineOrderCrossbowBolt.label</v>
@@ -4674,7 +4787,7 @@
         <v>사냥용 화살</v>
       </c>
     </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="101" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A101" s="1" t="str">
         <f t="shared" si="2"/>
         <v>ThingDef+BotchJob_DivineOrderHandCrossbow.label</v>
@@ -4696,7 +4809,7 @@
         <v>디바인 오더 한 손 석궁</v>
       </c>
     </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="102" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A102" s="1" t="str">
         <f t="shared" ref="A102" si="5">_xlfn.TEXTJOIN("+",,B102,C102)</f>
         <v>ThingDef+BotchJob_DivineOrderHandCrossbow.verbs.Verb_Shoot.label</v>
@@ -4716,7 +4829,7 @@
         <v>디바인 오더 한 손 석궁</v>
       </c>
     </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="103" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A103" s="1" t="str">
         <f t="shared" si="2"/>
         <v>ThingDef+BotchJob_DivineOrderHandCrossbow.description</v>
@@ -4738,7 +4851,7 @@
         <v>한 손에 들 수 있도록 설계된 작은 석궁입니다. 일반 석궁보다 사거리와 피해량은 적지만 발사 속도가 빠릅니다.</v>
       </c>
     </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="104" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A104" s="1" t="str">
         <f t="shared" si="2"/>
         <v>ThingDef+BotchJob_DivineOrderHandCrossbow.tools.0.label</v>
@@ -4760,7 +4873,7 @@
         <v>활대</v>
       </c>
     </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="105" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A105" s="1" t="str">
         <f t="shared" si="2"/>
         <v>ThingDef+BotchJob_DivineOrderHandCrossbowBolt.label</v>
@@ -4782,7 +4895,7 @@
         <v>석궁 볼트</v>
       </c>
     </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="106" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A106" s="1" t="str">
         <f t="shared" si="2"/>
         <v>ThingDef+BotchJob_DivineOrderCleansingConcoction.label</v>
@@ -4804,7 +4917,7 @@
         <v>정화용 혼합물</v>
       </c>
     </row>
-    <row r="107" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="107" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A107" s="1" t="str">
         <f t="shared" si="2"/>
         <v>ThingDef+BotchJob_DivineOrderCleansingConcoction.description</v>
@@ -4826,7 +4939,7 @@
         <v>봉인된 용기 안에 들어있는 불안정한 연금술 혼합물입니다. 불을 붙이고 던지면 몇 초 후 이글거리는 빛이 폭발하여 화상을 입거나 일시적으로 실명할 수 있습니다.\n\n디바인 오더 내에서 이 혼합물을 사용할 때는 타락한 것으로 간주되는 것을 정화"할 때입니다. 따라서 그 제조 방법은 철저히 비밀에 부쳐져 있습니다."</v>
       </c>
     </row>
-    <row r="108" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="108" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A108" s="1" t="str">
         <f t="shared" si="2"/>
         <v>ThingDef+BotchJob_DivineOrderCleansingConcoction.verbs.0.label</v>
@@ -4848,7 +4961,7 @@
         <v>혼합물 던지기</v>
       </c>
     </row>
-    <row r="109" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="109" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A109" s="1" t="str">
         <f t="shared" si="2"/>
         <v>ThingDef+BotchJob_DivineOrderCleansingConcoctionThrown.label</v>
@@ -4870,7 +4983,7 @@
         <v>정화용 혼합물</v>
       </c>
     </row>
-    <row r="110" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="110" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A110" s="1" t="str">
         <f t="shared" si="2"/>
         <v>PawnKindDef+BotchJob_DivineOrderHorse.label</v>
@@ -4892,7 +5005,7 @@
         <v>말</v>
       </c>
     </row>
-    <row r="111" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="111" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A111" s="1" t="str">
         <f t="shared" si="2"/>
         <v>PawnKindDef+BotchJob_DivineOrderHorse.labelMale</v>
@@ -4914,7 +5027,7 @@
         <v>종마</v>
       </c>
     </row>
-    <row r="112" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="112" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A112" s="1" t="str">
         <f t="shared" si="2"/>
         <v>PawnKindDef+BotchJob_DivineOrderHorse.labelFemale</v>
@@ -4936,7 +5049,7 @@
         <v>암말</v>
       </c>
     </row>
-    <row r="113" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="113" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A113" s="1" t="str">
         <f t="shared" si="2"/>
         <v>PawnKindDef+BotchJob_DivineOrderHorse.lifeStages.0.label</v>
@@ -4958,7 +5071,7 @@
         <v>망아지</v>
       </c>
     </row>
-    <row r="114" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="114" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A114" s="1" t="str">
         <f t="shared" si="2"/>
         <v>PawnKindDef+BotchJob_DivineOrderCommoner.label</v>
@@ -4980,7 +5093,7 @@
         <v>평민</v>
       </c>
     </row>
-    <row r="115" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="115" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A115" s="1" t="str">
         <f t="shared" si="2"/>
         <v>PawnKindDef+BotchJob_DivineOrderMerchant.label</v>
@@ -5002,7 +5115,7 @@
         <v>상인</v>
       </c>
     </row>
-    <row r="116" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="116" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A116" s="1" t="str">
         <f t="shared" si="2"/>
         <v>PawnKindDef+BotchJob_DivineOrderConscript.label</v>
@@ -5024,7 +5137,7 @@
         <v>징집병</v>
       </c>
     </row>
-    <row r="117" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="117" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A117" s="1" t="str">
         <f t="shared" si="2"/>
         <v>PawnKindDef+BotchJob_DivineOrderStandardBearer.label</v>
@@ -5046,7 +5159,7 @@
         <v>기수</v>
       </c>
     </row>
-    <row r="118" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="118" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A118" s="1" t="str">
         <f t="shared" si="2"/>
         <v>PawnKindDef+BotchJob_DivineOrderScout.label</v>
@@ -5068,7 +5181,7 @@
         <v>스카우트</v>
       </c>
     </row>
-    <row r="119" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="119" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A119" s="1" t="str">
         <f t="shared" si="2"/>
         <v>PawnKindDef+BotchJob_DivineOrderFighter.label</v>
@@ -5090,7 +5203,7 @@
         <v>파이터</v>
       </c>
     </row>
-    <row r="120" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="120" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A120" s="1" t="str">
         <f t="shared" si="2"/>
         <v>PawnKindDef+BotchJob_DivineOrderZealot.label</v>
@@ -5112,7 +5225,7 @@
         <v>광신도</v>
       </c>
     </row>
-    <row r="121" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="121" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A121" s="1" t="str">
         <f t="shared" si="2"/>
         <v>PawnKindDef+BotchJob_DivineOrderSharpshooter.label</v>
@@ -5134,7 +5247,7 @@
         <v>샤프슈터</v>
       </c>
     </row>
-    <row r="122" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="122" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A122" s="1" t="str">
         <f t="shared" si="2"/>
         <v>PawnKindDef+BotchJob_DivineOrderKnight.label</v>
@@ -5156,7 +5269,7 @@
         <v>나이트</v>
       </c>
     </row>
-    <row r="123" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="123" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A123" s="1" t="str">
         <f t="shared" si="2"/>
         <v>PawnKindDef+BotchJob_DivineOrderChampion.label</v>
@@ -5178,7 +5291,7 @@
         <v>챔피언</v>
       </c>
     </row>
-    <row r="124" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="124" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A124" s="1" t="str">
         <f t="shared" si="2"/>
         <v>PawnKindDef+BotchJob_DivineOrderCrusader.label</v>
@@ -5200,7 +5313,7 @@
         <v>크루세이더</v>
       </c>
     </row>
-    <row r="125" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="125" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A125" s="1" t="str">
         <f t="shared" si="2"/>
         <v>PawnKindDef+BotchJob_DivineOrderInquisitor.label</v>
@@ -5222,7 +5335,7 @@
         <v>인퀴지터</v>
       </c>
     </row>
-    <row r="126" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="126" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A126" s="1" t="str">
         <f t="shared" si="2"/>
         <v>PawnKindDef+BotchJob_DivineOrderHerald.label</v>
@@ -5244,7 +5357,7 @@
         <v>헤럴드</v>
       </c>
     </row>
-    <row r="127" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="127" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A127" s="1" t="str">
         <f t="shared" si="2"/>
         <v>PawnKindDef+BotchJob_DivineOrderDefector.label</v>
@@ -5266,7 +5379,7 @@
         <v>탈주자</v>
       </c>
     </row>
-    <row r="128" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="128" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A128" s="1" t="str">
         <f t="shared" si="2"/>
         <v>BackstoryDef+BotchJobDivineOrder_Chosen.title</v>
@@ -5288,7 +5401,7 @@
         <v>고귀한 자들에게 선택받은 자</v>
       </c>
     </row>
-    <row r="129" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="129" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A129" s="1" t="str">
         <f t="shared" si="2"/>
         <v>BackstoryDef+BotchJobDivineOrder_Chosen.titleShort</v>
@@ -5310,7 +5423,7 @@
         <v>선택받은 자</v>
       </c>
     </row>
-    <row r="130" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="130" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A130" s="1" t="str">
         <f t="shared" si="2"/>
         <v>BackstoryDef+BotchJobDivineOrder_Chosen.baseDesc</v>
@@ -5332,7 +5445,7 @@
         <v>[PAWN_nameDef](은)는 어린 나이에 선택되어 육체적, 정신적 강인함을 극한까지 밀어붙이는 잔혹한 훈련인 고귀한 자들의 시련을 겪었습니다. 시련에서 살아남는 사람은 극소수에 불과하지만, 살아남은 사람은 크루세이더, 인퀴지터 또는 디바인 오더의 헤럴드로 성장합니다.</v>
       </c>
     </row>
-    <row r="131" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="131" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A131" s="1" t="str">
         <f t="shared" si="2"/>
         <v>BackstoryDef+BotchJobDivineOrder_Crusader.title</v>
@@ -5354,7 +5467,7 @@
         <v>디바인 오더 크루세이더</v>
       </c>
     </row>
-    <row r="132" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="132" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A132" s="1" t="str">
         <f t="shared" si="2"/>
         <v>BackstoryDef+BotchJobDivineOrder_Crusader.titleShort</v>
@@ -5376,7 +5489,7 @@
         <v>크루세이더</v>
       </c>
     </row>
-    <row r="133" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="133" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A133" s="1" t="str">
         <f t="shared" si="2"/>
         <v>BackstoryDef+BotchJobDivineOrder_Crusader.baseDesc</v>
@@ -5398,7 +5511,7 @@
         <v>[PAWN_nameDef](은)는 고귀한 자들의 시련에서 살아남아 디바인 오더의 크루세이더로 성장했습니다.</v>
       </c>
     </row>
-    <row r="134" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="134" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A134" s="1" t="str">
         <f t="shared" si="2"/>
         <v>BackstoryDef+BotchJobDivineOrder_Inquisitor.title</v>
@@ -5420,7 +5533,7 @@
         <v>디바인 오더 인퀴지터</v>
       </c>
     </row>
-    <row r="135" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="135" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A135" s="1" t="str">
         <f t="shared" si="2"/>
         <v>BackstoryDef+BotchJobDivineOrder_Inquisitor.titleShort</v>
@@ -5442,7 +5555,7 @@
         <v>인퀴지터</v>
       </c>
     </row>
-    <row r="136" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="136" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A136" s="1" t="str">
         <f t="shared" ref="A136:A167" si="6">_xlfn.TEXTJOIN("+",,B136,C136)</f>
         <v>BackstoryDef+BotchJobDivineOrder_Inquisitor.baseDesc</v>
@@ -5464,7 +5577,7 @@
         <v>[PAWN_nameDef](은)는 고귀한 자들의 시련에서 살아남아 디바인 오더의 인퀴지터로 성장했습니다.</v>
       </c>
     </row>
-    <row r="137" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="137" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A137" s="1" t="str">
         <f t="shared" si="6"/>
         <v>BackstoryDef+BotchJobDivineOrder_Herald.title</v>
@@ -5486,7 +5599,7 @@
         <v>디바인 오더 헤럴드</v>
       </c>
     </row>
-    <row r="138" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="138" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A138" s="1" t="str">
         <f t="shared" si="6"/>
         <v>BackstoryDef+BotchJobDivineOrder_Herald.titleShort</v>
@@ -5508,7 +5621,7 @@
         <v>헤럴드</v>
       </c>
     </row>
-    <row r="139" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="139" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A139" s="1" t="str">
         <f t="shared" si="6"/>
         <v>BackstoryDef+BotchJobDivineOrder_Herald.baseDesc</v>
@@ -5530,7 +5643,7 @@
         <v>[PAWN_nameDef](은)는 고귀한 자들의 시련에서 살아남아 디바인 오더의 헤럴드로 성장했습니다.</v>
       </c>
     </row>
-    <row r="140" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="140" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A140" s="1" t="str">
         <f t="shared" si="6"/>
         <v>FactionDef+BotchJob_DivineOrderFaction.label</v>
@@ -5552,7 +5665,7 @@
         <v>디바인 오더</v>
       </c>
     </row>
-    <row r="141" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="141" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A141" s="1" t="str">
         <f t="shared" si="6"/>
         <v>FactionDef+BotchJob_DivineOrderFaction.description</v>
@@ -5574,7 +5687,7 @@
         <v>교단에 강제로 들어왔든 태어날 때부터 믿었든 간에 이들은 투철한 신념을 가졌으며, 부패한 영역을 정화하는 것을 신성한 사명으로 여깁니다. 외부인을 매우 불신하지만 이유 없이 불신하는 것은 아니며, 이익이 된다면 어색하게나마 동맹을 맺는 것으로 알려져 있습니다.</v>
       </c>
     </row>
-    <row r="142" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="142" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A142" s="1" t="str">
         <f t="shared" ref="A142" si="7">_xlfn.TEXTJOIN("+",,B142,C142)</f>
         <v>FactionDef+BotchJob_DivineOrderFaction.fixedName</v>
@@ -5583,10 +5696,10 @@
         <v>396</v>
       </c>
       <c r="C142" s="1" t="s">
-        <v>652</v>
+        <v>650</v>
       </c>
       <c r="D142" s="1" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
       <c r="E142" s="1" t="s">
         <v>487</v>
@@ -5596,7 +5709,7 @@
         <v>디바인 오더</v>
       </c>
     </row>
-    <row r="143" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="143" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A143" s="1" t="str">
         <f t="shared" si="6"/>
         <v>FactionDef+BotchJob_DivineOrderFaction.pawnSingular</v>
@@ -5618,7 +5731,7 @@
         <v>추종자</v>
       </c>
     </row>
-    <row r="144" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="144" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A144" s="1" t="str">
         <f t="shared" si="6"/>
         <v>FactionDef+BotchJob_DivineOrderFaction.pawnsPlural</v>
@@ -5640,7 +5753,7 @@
         <v>추종자들</v>
       </c>
     </row>
-    <row r="145" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="145" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A145" s="1" t="str">
         <f t="shared" si="6"/>
         <v>FactionDef+BotchJob_DivineOrderFaction.leaderTitle</v>
@@ -5662,7 +5775,7 @@
         <v>로드 커맨더</v>
       </c>
     </row>
-    <row r="146" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="146" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A146" s="1" t="str">
         <f t="shared" si="6"/>
         <v>FactionDef+BotchJob_DivineOrderPlayerFaction.label</v>
@@ -5684,7 +5797,7 @@
         <v>디바인 오더 탈주자</v>
       </c>
     </row>
-    <row r="147" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="147" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A147" s="1" t="str">
         <f t="shared" si="6"/>
         <v>FactionDef+BotchJob_DivineOrderPlayerFaction.description</v>
@@ -5706,7 +5819,7 @@
         <v>디바인 오더에서 탈출한 소수의 망명자 집단입니다.</v>
       </c>
     </row>
-    <row r="148" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="148" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A148" s="1" t="str">
         <f t="shared" si="6"/>
         <v>FactionDef+BotchJob_DivineOrderPlayerFaction.pawnSingular</v>
@@ -5728,7 +5841,7 @@
         <v>탈주자</v>
       </c>
     </row>
-    <row r="149" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="149" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A149" s="1" t="str">
         <f t="shared" si="6"/>
         <v>FactionDef+BotchJob_DivineOrderPlayerFaction.pawnsPlural</v>
@@ -5750,7 +5863,7 @@
         <v>탈주자들</v>
       </c>
     </row>
-    <row r="150" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="150" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A150" s="1" t="str">
         <f t="shared" si="6"/>
         <v>ResearchProjectDef+BotchJob_DivineOrderSmithing.label</v>
@@ -5772,7 +5885,7 @@
         <v>디바인 오더 장비</v>
       </c>
     </row>
-    <row r="151" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="151" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A151" s="1" t="str">
         <f t="shared" si="6"/>
         <v>ResearchProjectDef+BotchJob_DivineOrderSmithing.description</v>
@@ -5794,7 +5907,7 @@
         <v>디바인 오더의 기본 무기, 방어구, 의복 제작하는 법을 배웁니다.</v>
       </c>
     </row>
-    <row r="152" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="152" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A152" s="1" t="str">
         <f t="shared" si="6"/>
         <v>ResearchProjectDef+BotchJob_DivineOrderEliteArmor.label</v>
@@ -5816,7 +5929,7 @@
         <v>디바인 오더 엘리트 아머</v>
       </c>
     </row>
-    <row r="153" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="153" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A153" s="1" t="str">
         <f t="shared" si="6"/>
         <v>ResearchProjectDef+BotchJob_DivineOrderEliteArmor.description</v>
@@ -5838,7 +5951,7 @@
         <v>디바인 오더의 크루세이더, 인퀴지터, 헤럴드가 착용하는 강력한 갑옷의 제작 방법을 배웁니다.</v>
       </c>
     </row>
-    <row r="154" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="154" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A154" s="1" t="str">
         <f t="shared" si="6"/>
         <v>ScenarioDef+BotchJob_DivineOrderStart.scenario.name</v>
@@ -5860,7 +5973,7 @@
         <v>디바인 오더 탈주자들</v>
       </c>
     </row>
-    <row r="155" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="155" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A155" s="1" t="str">
         <f t="shared" si="6"/>
         <v>ScenarioDef+BotchJob_DivineOrderStart.scenario.description</v>
@@ -5882,7 +5995,7 @@
         <v>디바인 오더의 수련생이었던 네 사람은 탈영하여 몇 주 동안 도망 다니고 있습니다.\n\n보급품은 바닥나고, 기본적인 장비와 말 한 마리밖에 없지만, 그나마 한 가지 다행인 것은 오더에서 그토록 숭배하는 성스러운 석판이 아직 남아 있다는 것입니다. 적절한 구매자로부터 상당한 금액을 받을 수도 있고, 아니면 당신이 가지고 있으면서 그 비밀을 밝혀낼 수도 있습니다.\n\n어느 쪽이든 영원히 도망칠 수는 없습니다. 지금은 안정을 취하고 앞으로 다가올 도전에 맞설 준비를 하기에 가장 좋은 시기입니다. 쉽지는 않겠지만 희망과 근성이 있다면 여러분은 새로운 삶을 개척할 수 있을지도 모릅니다.\n\n한 가지 확실한 것은, 결국 오더가 당신을 찾아낼 것이고 그들은 자비를 베풀지 않을 것이라는 점입니다.\n\n준비해야 합니다.</v>
       </c>
     </row>
-    <row r="156" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="156" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A156" s="1" t="str">
         <f t="shared" si="6"/>
         <v>ScenarioDef+BotchJob_DivineOrderStart.scenario.summary</v>
@@ -5904,7 +6017,7 @@
         <v>디바인 오더에서 도망친 네 명의 탈주자.</v>
       </c>
     </row>
-    <row r="157" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="157" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A157" s="1" t="str">
         <f t="shared" si="6"/>
         <v>ScenarioDef+BotchJob_DivineOrderStart.scenario.parts.GameStartDialog.text</v>
@@ -5926,7 +6039,7 @@
         <v>네 사람은 디바인 오더에서 탈영하여 몇 주 동안 도망 다녔고, 다행히도 지금은 교단의 눈을 피해 도망친 것 같습니다.\n\n보급품은 바닥을 드러내고 있고 기본적인 장비와 말 한 마리밖에 없지만 그나마 한 가지 다행인 것은 신성한 석판이 아직 남아 있다는 점입니다. 적절한 구매자로부터 상당한 금액을 받을 수도 있고, 아니면 당신이 가지고 있으면서 그 비밀을 밝혀낼 수도 있습니다.\n\n어느 쪽이든 영원히 도망칠 수는 없습니다. 지금은 안정을 취하고 앞으로 다가올 도전에 맞설 준비를 하기에 가장 좋은 시기입니다. 쉽지는 않겠지만 희망과 근성이 있다면 여러분은 새로운 삶을 개척할 수 있을지도 모릅니다.\n\n한 가지 확실한 것은, 결국 오더가 당신을 찾아낼 것이고 그들은 자비를 베풀지 않을 것이라는 점입니다.\n\n준비해야 합니다.</v>
       </c>
     </row>
-    <row r="158" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="158" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A158" s="1" t="str">
         <f t="shared" si="6"/>
         <v>CultureDef+BotchJob_DivineOrderCulture.label</v>
@@ -5948,7 +6061,7 @@
         <v>디바인 오더</v>
       </c>
     </row>
-    <row r="159" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="159" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A159" s="1" t="str">
         <f t="shared" si="6"/>
         <v>CultureDef+BotchJob_DivineOrderCulture.description</v>
@@ -5970,7 +6083,7 @@
         <v>교단에 강제로 들어왔든 태어날 때부터 믿었든 간에 이들은 투철한 신념을 가졌으며, 부패한 영역을 정화하는 것을 신성한 사명으로 여깁니다. 외부인을 매우 불신하지만 이유 없이 불신하는 것은 아니며, 이익이 된다면 어색하게나마 동맹을 맺는 것으로 알려져 있습니다.</v>
       </c>
     </row>
-    <row r="160" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="160" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A160" s="1" t="str">
         <f t="shared" si="6"/>
         <v>StyleCategoryDef+BotchJob_DivineOrderStyleCategory.label</v>
@@ -5992,7 +6105,7 @@
         <v>디바인 오더</v>
       </c>
     </row>
-    <row r="161" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="161" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A161" s="1" t="str">
         <f t="shared" si="6"/>
         <v>TraderKindDef+BotchJob_DivineOrderCaravanTrader.label</v>
@@ -6014,7 +6127,7 @@
         <v>디바인 오더 상인</v>
       </c>
     </row>
-    <row r="162" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="162" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A162" s="1" t="str">
         <f t="shared" si="6"/>
         <v>TraderKindDef+BotchJob_DivineOrderVisitor.label</v>
@@ -6036,7 +6149,7 @@
         <v>상인</v>
       </c>
     </row>
-    <row r="163" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="163" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A163" s="1" t="str">
         <f t="shared" si="6"/>
         <v>DamageDef+BotchJob_DivineOrderCleansingBlast.label</v>
@@ -6058,7 +6171,7 @@
         <v>정화의 폭풍</v>
       </c>
     </row>
-    <row r="164" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="164" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A164" s="1" t="str">
         <f t="shared" si="6"/>
         <v>DamageDef+BotchJob_DivineOrderCleansingBlast.deathMessage</v>
@@ -6080,7 +6193,7 @@
         <v>{0}(이)가 정화 되었습니다.</v>
       </c>
     </row>
-    <row r="165" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="165" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A165" s="1" t="str">
         <f t="shared" si="6"/>
         <v>HediffDef+BotchJob_BlindingFlash.label</v>
@@ -6102,7 +6215,7 @@
         <v>눈부신 빛</v>
       </c>
     </row>
-    <row r="166" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="166" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A166" s="1" t="str">
         <f t="shared" si="6"/>
         <v>HediffDef+BotchJob_BlindingFlash.labelNoun</v>
@@ -6124,7 +6237,7 @@
         <v>섬광</v>
       </c>
     </row>
-    <row r="167" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="167" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A167" s="1" t="str">
         <f t="shared" si="6"/>
         <v>HediffDef+BotchJob_BlindingFlash.description</v>
@@ -6146,19 +6259,19 @@
         <v>눈부신 빛에 노출되면 일시적인 시력 장애가 발생할 수 있습니다.</v>
       </c>
     </row>
-    <row r="168" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="168" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A168" s="1" t="str">
-        <f t="shared" ref="A168" si="8">_xlfn.TEXTJOIN("+",,B168,C168)</f>
+        <f t="shared" ref="A168:A180" si="8">_xlfn.TEXTJOIN("+",,B168,C168)</f>
         <v>HediffDef+BotchJob_BlindingFlash.battleStateLabel</v>
       </c>
       <c r="B168" s="1" t="s">
         <v>466</v>
       </c>
       <c r="C168" s="1" t="s">
-        <v>655</v>
+        <v>653</v>
       </c>
       <c r="D168" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
       <c r="E168" t="s">
         <v>505</v>
@@ -6166,6 +6279,285 @@
       <c r="G168" t="str">
         <f>IFERROR(VLOOKUP(A168,Update!$C$2:$D$173,2,FALSE),"")</f>
         <v>눈이 멈</v>
+      </c>
+    </row>
+    <row r="169" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A169" s="1" t="str">
+        <f t="shared" si="8"/>
+        <v>DamageDef+BotchJob_DivineOrderStaffBlast.label</v>
+      </c>
+      <c r="B169" t="s">
+        <v>459</v>
+      </c>
+      <c r="C169" t="s">
+        <v>664</v>
+      </c>
+      <c r="D169" t="s">
+        <v>673</v>
+      </c>
+      <c r="E169" s="1" t="s">
+        <v>679</v>
+      </c>
+      <c r="G169" t="s">
+        <v>655</v>
+      </c>
+      <c r="H169" t="str">
+        <f>MID(G169,FIND("'",G169)+1,FIND("'",G169,FIND("'",G169)+1)-FIND("'",G169)-1)</f>
+        <v>divine judgement</v>
+      </c>
+    </row>
+    <row r="170" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A170" s="1" t="str">
+        <f t="shared" si="8"/>
+        <v>DamageDef+BotchJob_DivineOrderStaffBlast.deathMessage</v>
+      </c>
+      <c r="B170" t="s">
+        <v>459</v>
+      </c>
+      <c r="C170" t="s">
+        <v>665</v>
+      </c>
+      <c r="D170" t="s">
+        <v>674</v>
+      </c>
+      <c r="E170" t="s">
+        <v>680</v>
+      </c>
+      <c r="G170" t="s">
+        <v>656</v>
+      </c>
+      <c r="H170" t="str">
+        <f t="shared" ref="H170:H177" si="9">MID(G170,FIND("'",G170)+1,FIND("'",G170,FIND("'",G170)+1)-FIND("'",G170)-1)</f>
+        <v>{0} has been incinerated by divine light.</v>
+      </c>
+    </row>
+    <row r="171" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A171" s="1" t="str">
+        <f t="shared" si="8"/>
+        <v>ResearchProjectDef+BotchJob_DivineOrderStaffResearch.label</v>
+      </c>
+      <c r="B171" t="s">
+        <v>423</v>
+      </c>
+      <c r="C171" t="s">
+        <v>666</v>
+      </c>
+      <c r="D171" t="s">
+        <v>675</v>
+      </c>
+      <c r="E171" s="1" t="s">
+        <v>681</v>
+      </c>
+      <c r="G171" t="s">
+        <v>657</v>
+      </c>
+      <c r="H171" t="str">
+        <f t="shared" si="9"/>
+        <v>staff of divine judgement</v>
+      </c>
+    </row>
+    <row r="172" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A172" s="1" t="str">
+        <f t="shared" si="8"/>
+        <v>ResearchProjectDef+BotchJob_DivineOrderStaffResearch.description</v>
+      </c>
+      <c r="B172" t="s">
+        <v>423</v>
+      </c>
+      <c r="C172" t="s">
+        <v>667</v>
+      </c>
+      <c r="D172" t="s">
+        <v>676</v>
+      </c>
+      <c r="E172" t="s">
+        <v>682</v>
+      </c>
+      <c r="G172" t="s">
+        <v>658</v>
+      </c>
+      <c r="H172" t="str">
+        <f t="shared" si="9"/>
+        <v>Learn to craft the staff of divine judgement, the ultimate weapon of the divine order.</v>
+      </c>
+    </row>
+    <row r="173" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A173" s="1" t="str">
+        <f t="shared" si="8"/>
+        <v>ThingDef+BotchJob_DivineJudgementStaff.label</v>
+      </c>
+      <c r="B173" t="s">
+        <v>7</v>
+      </c>
+      <c r="C173" t="s">
+        <v>668</v>
+      </c>
+      <c r="D173" t="s">
+        <v>675</v>
+      </c>
+      <c r="E173" s="1" t="s">
+        <v>681</v>
+      </c>
+      <c r="G173" t="s">
+        <v>659</v>
+      </c>
+      <c r="H173" t="str">
+        <f t="shared" si="9"/>
+        <v>staff of divine judgement</v>
+      </c>
+    </row>
+    <row r="174" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A174" s="1" t="str">
+        <f t="shared" si="8"/>
+        <v>ThingDef+BotchJob_DivineJudgementStaff.description</v>
+      </c>
+      <c r="B174" t="s">
+        <v>7</v>
+      </c>
+      <c r="C174" t="s">
+        <v>669</v>
+      </c>
+      <c r="D174" t="s">
+        <v>677</v>
+      </c>
+      <c r="E174" t="s">
+        <v>683</v>
+      </c>
+      <c r="G174" t="s">
+        <v>660</v>
+      </c>
+      <c r="H174" t="str">
+        <f t="shared" si="9"/>
+        <v>The ultimate weapon of the Divine order. A grand, ornate staff that radiates divine power.\n\nWielding this staff grants the ability to call upon the power of the gods to deliver divine judgement, devastating an area with cleansing light.</v>
+      </c>
+    </row>
+    <row r="175" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A175" s="1" t="str">
+        <f t="shared" si="8"/>
+        <v>ThingDef+BotchJob_DivineJudgementStaff.tools.shaft.label</v>
+      </c>
+      <c r="B175" t="s">
+        <v>7</v>
+      </c>
+      <c r="C175" t="s">
+        <v>670</v>
+      </c>
+      <c r="D175" t="s">
+        <v>236</v>
+      </c>
+      <c r="E175" s="1" t="s">
+        <v>684</v>
+      </c>
+      <c r="G175" t="s">
+        <v>661</v>
+      </c>
+      <c r="H175" t="str">
+        <f t="shared" si="9"/>
+        <v>shaft</v>
+      </c>
+    </row>
+    <row r="176" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A176" s="1" t="str">
+        <f t="shared" si="8"/>
+        <v>ThingDef+BotchJob_DivineJudgementStaff.verbs.divine_judgement.label</v>
+      </c>
+      <c r="B176" t="s">
+        <v>7</v>
+      </c>
+      <c r="C176" t="s">
+        <v>671</v>
+      </c>
+      <c r="D176" t="s">
+        <v>673</v>
+      </c>
+      <c r="E176" s="1" t="s">
+        <v>679</v>
+      </c>
+      <c r="G176" t="s">
+        <v>662</v>
+      </c>
+      <c r="H176" t="str">
+        <f t="shared" si="9"/>
+        <v>divine judgement</v>
+      </c>
+    </row>
+    <row r="177" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A177" s="1" t="str">
+        <f t="shared" si="8"/>
+        <v>ThingDef+BotchJob_DivineOrderStaffThrown.label</v>
+      </c>
+      <c r="B177" t="s">
+        <v>7</v>
+      </c>
+      <c r="C177" t="s">
+        <v>672</v>
+      </c>
+      <c r="D177" t="s">
+        <v>678</v>
+      </c>
+      <c r="E177" s="1" t="s">
+        <v>685</v>
+      </c>
+      <c r="G177" t="s">
+        <v>663</v>
+      </c>
+      <c r="H177" t="str">
+        <f t="shared" si="9"/>
+        <v>divine blast</v>
+      </c>
+    </row>
+    <row r="178" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A178" s="1" t="str">
+        <f t="shared" si="8"/>
+        <v>FactionDef+BotchJob_DivineOrderPlayerFaction.leaderTitle</v>
+      </c>
+      <c r="B178" t="s">
+        <v>396</v>
+      </c>
+      <c r="C178" t="s">
+        <v>686</v>
+      </c>
+      <c r="D178" t="s">
+        <v>687</v>
+      </c>
+      <c r="E178" s="1" t="s">
+        <v>692</v>
+      </c>
+    </row>
+    <row r="179" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A179" s="1" t="str">
+        <f t="shared" si="8"/>
+        <v>ScenarioDef+BotchJob_DivineOrderStart.label</v>
+      </c>
+      <c r="B179" t="s">
+        <v>435</v>
+      </c>
+      <c r="C179" t="s">
+        <v>688</v>
+      </c>
+      <c r="D179" t="s">
+        <v>413</v>
+      </c>
+      <c r="E179" s="1" t="s">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="180" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A180" s="1" t="str">
+        <f t="shared" si="8"/>
+        <v>ScenarioDef+BotchJob_DivineOrderStart.description</v>
+      </c>
+      <c r="B180" t="s">
+        <v>435</v>
+      </c>
+      <c r="C180" t="s">
+        <v>689</v>
+      </c>
+      <c r="D180" t="s">
+        <v>438</v>
+      </c>
+      <c r="E180" s="1" t="s">
+        <v>527</v>
       </c>
     </row>
   </sheetData>
@@ -6178,19 +6570,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52B24FAC-7C75-4A19-A409-F75EAD5D64F8}">
   <dimension ref="A1:E173"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+    <sheetView topLeftCell="A145" workbookViewId="0">
+      <selection activeCell="E169" sqref="E169"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="69.4140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="69.375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="51.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="69.4140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="69.375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="32.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>636</v>
       </c>
@@ -6201,7 +6593,7 @@
         <v>637</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>368</v>
       </c>
@@ -6217,7 +6609,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>361</v>
       </c>
@@ -6233,7 +6625,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>365</v>
       </c>
@@ -6249,7 +6641,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>376</v>
       </c>
@@ -6265,7 +6657,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>371</v>
       </c>
@@ -6281,7 +6673,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>374</v>
       </c>
@@ -6297,7 +6689,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>384</v>
       </c>
@@ -6313,7 +6705,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>379</v>
       </c>
@@ -6329,7 +6721,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>382</v>
       </c>
@@ -6345,7 +6737,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>392</v>
       </c>
@@ -6361,7 +6753,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>387</v>
       </c>
@@ -6377,7 +6769,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>390</v>
       </c>
@@ -6393,7 +6785,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>443</v>
       </c>
@@ -6409,7 +6801,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>446</v>
       </c>
@@ -6425,7 +6817,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>458</v>
       </c>
@@ -6441,7 +6833,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>462</v>
       </c>
@@ -6457,7 +6849,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>395</v>
       </c>
@@ -6473,7 +6865,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>399</v>
       </c>
@@ -6489,7 +6881,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>491</v>
       </c>
@@ -6505,7 +6897,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>402</v>
       </c>
@@ -6521,7 +6913,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>405</v>
       </c>
@@ -6537,7 +6929,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>408</v>
       </c>
@@ -6553,7 +6945,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>411</v>
       </c>
@@ -6569,7 +6961,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>414</v>
       </c>
@@ -6585,7 +6977,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>497</v>
       </c>
@@ -6601,7 +6993,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>417</v>
       </c>
@@ -6617,7 +7009,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>419</v>
       </c>
@@ -6633,7 +7025,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>465</v>
       </c>
@@ -6649,7 +7041,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>469</v>
       </c>
@@ -6665,7 +7057,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>472</v>
       </c>
@@ -6681,7 +7073,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>504</v>
       </c>
@@ -6697,7 +7089,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>308</v>
       </c>
@@ -6713,7 +7105,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>310</v>
       </c>
@@ -6729,7 +7121,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>313</v>
       </c>
@@ -6745,7 +7137,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>316</v>
       </c>
@@ -6761,7 +7153,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>319</v>
       </c>
@@ -6777,7 +7169,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>322</v>
       </c>
@@ -6793,7 +7185,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>325</v>
       </c>
@@ -6809,7 +7201,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>328</v>
       </c>
@@ -6825,7 +7217,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>331</v>
       </c>
@@ -6841,7 +7233,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>334</v>
       </c>
@@ -6857,7 +7249,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>340</v>
       </c>
@@ -6873,7 +7265,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>343</v>
       </c>
@@ -6889,7 +7281,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>346</v>
       </c>
@@ -6905,7 +7297,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>349</v>
       </c>
@@ -6921,7 +7313,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>352</v>
       </c>
@@ -6937,7 +7329,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>355</v>
       </c>
@@ -6953,7 +7345,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>337</v>
       </c>
@@ -6969,7 +7361,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>358</v>
       </c>
@@ -6985,7 +7377,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>422</v>
       </c>
@@ -7001,7 +7393,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>426</v>
       </c>
@@ -7017,7 +7409,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>429</v>
       </c>
@@ -7033,7 +7425,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>432</v>
       </c>
@@ -7049,7 +7441,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>524</v>
       </c>
@@ -7069,7 +7461,7 @@
         <v/>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>526</v>
       </c>
@@ -7089,7 +7481,7 @@
         <v/>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>436</v>
       </c>
@@ -7105,7 +7497,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>528</v>
       </c>
@@ -7121,7 +7513,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>640</v>
       </c>
@@ -7137,7 +7529,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>439</v>
       </c>
@@ -7153,7 +7545,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>448</v>
       </c>
@@ -7169,7 +7561,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>6</v>
       </c>
@@ -7185,7 +7577,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>11</v>
       </c>
@@ -7201,7 +7593,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>15</v>
       </c>
@@ -7217,7 +7609,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>19</v>
       </c>
@@ -7233,7 +7625,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>23</v>
       </c>
@@ -7249,7 +7641,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>26</v>
       </c>
@@ -7265,7 +7657,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>29</v>
       </c>
@@ -7281,7 +7673,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>32</v>
       </c>
@@ -7297,7 +7689,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>35</v>
       </c>
@@ -7313,7 +7705,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>38</v>
       </c>
@@ -7329,7 +7721,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>47</v>
       </c>
@@ -7345,7 +7737,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>50</v>
       </c>
@@ -7361,7 +7753,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>59</v>
       </c>
@@ -7377,7 +7769,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>62</v>
       </c>
@@ -7393,7 +7785,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>65</v>
       </c>
@@ -7409,7 +7801,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>68</v>
       </c>
@@ -7425,7 +7817,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>71</v>
       </c>
@@ -7441,7 +7833,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>74</v>
       </c>
@@ -7457,7 +7849,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>77</v>
       </c>
@@ -7473,7 +7865,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>80</v>
       </c>
@@ -7489,7 +7881,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>83</v>
       </c>
@@ -7505,7 +7897,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>86</v>
       </c>
@@ -7521,7 +7913,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>89</v>
       </c>
@@ -7537,7 +7929,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>92</v>
       </c>
@@ -7553,7 +7945,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>95</v>
       </c>
@@ -7569,7 +7961,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>98</v>
       </c>
@@ -7585,7 +7977,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>101</v>
       </c>
@@ -7601,7 +7993,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>104</v>
       </c>
@@ -7617,7 +8009,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>107</v>
       </c>
@@ -7633,7 +8025,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>110</v>
       </c>
@@ -7649,7 +8041,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>113</v>
       </c>
@@ -7665,7 +8057,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>116</v>
       </c>
@@ -7681,7 +8073,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>119</v>
       </c>
@@ -7697,7 +8089,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>122</v>
       </c>
@@ -7713,7 +8105,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>125</v>
       </c>
@@ -7729,7 +8121,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>128</v>
       </c>
@@ -7745,7 +8137,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>131</v>
       </c>
@@ -7761,7 +8153,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>134</v>
       </c>
@@ -7777,7 +8169,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
         <v>137</v>
       </c>
@@ -7793,7 +8185,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="101" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
         <v>140</v>
       </c>
@@ -7809,7 +8201,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="102" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
         <v>143</v>
       </c>
@@ -7825,7 +8217,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="103" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
         <v>146</v>
       </c>
@@ -7841,7 +8233,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="104" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
         <v>149</v>
       </c>
@@ -7857,7 +8249,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="105" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
         <v>152</v>
       </c>
@@ -7873,7 +8265,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="106" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
         <v>155</v>
       </c>
@@ -7889,7 +8281,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="107" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
         <v>158</v>
       </c>
@@ -7905,7 +8297,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="108" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
         <v>161</v>
       </c>
@@ -7921,7 +8313,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="109" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
         <v>164</v>
       </c>
@@ -7937,7 +8329,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="110" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
         <v>167</v>
       </c>
@@ -7953,7 +8345,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="111" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
         <v>170</v>
       </c>
@@ -7969,7 +8361,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="112" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
         <v>173</v>
       </c>
@@ -7985,7 +8377,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="113" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
         <v>176</v>
       </c>
@@ -8001,7 +8393,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="114" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
         <v>179</v>
       </c>
@@ -8017,7 +8409,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="115" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
         <v>182</v>
       </c>
@@ -8033,7 +8425,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="116" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
         <v>185</v>
       </c>
@@ -8049,7 +8441,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="117" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
         <v>188</v>
       </c>
@@ -8065,12 +8457,12 @@
         <v>60</v>
       </c>
     </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="118" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
         <v>587</v>
       </c>
       <c r="B118" s="1" t="s">
-        <v>650</v>
+        <v>648</v>
       </c>
       <c r="C118" t="str">
         <f t="shared" si="1"/>
@@ -8079,17 +8471,17 @@
       <c r="D118" t="s">
         <v>588</v>
       </c>
-      <c r="E118">
+      <c r="E118" t="e">
         <f>IF(ISERROR(B118),"",MATCH(C118,Sheet!$A$2:$A$168,0))</f>
-        <v>61</v>
-      </c>
-    </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.45">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="119" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
         <v>589</v>
       </c>
       <c r="B119" s="1" t="s">
-        <v>651</v>
+        <v>649</v>
       </c>
       <c r="C119" t="str">
         <f t="shared" si="1"/>
@@ -8098,12 +8490,12 @@
       <c r="D119" t="s">
         <v>590</v>
       </c>
-      <c r="E119">
+      <c r="E119" t="e">
         <f>IF(ISERROR(B119),"",MATCH(C119,Sheet!$A$2:$A$168,0))</f>
-        <v>62</v>
-      </c>
-    </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.45">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
         <v>191</v>
       </c>
@@ -8119,7 +8511,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="121" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
         <v>194</v>
       </c>
@@ -8135,7 +8527,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="122" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
         <v>197</v>
       </c>
@@ -8151,7 +8543,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="123" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
         <v>200</v>
       </c>
@@ -8167,7 +8559,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="124" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
         <v>202</v>
       </c>
@@ -8183,7 +8575,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="125" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
         <v>205</v>
       </c>
@@ -8199,7 +8591,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="126" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
         <v>208</v>
       </c>
@@ -8215,7 +8607,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="127" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
         <v>210</v>
       </c>
@@ -8231,7 +8623,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="128" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
         <v>213</v>
       </c>
@@ -8247,7 +8639,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="129" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
         <v>216</v>
       </c>
@@ -8263,7 +8655,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="130" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
         <v>219</v>
       </c>
@@ -8279,7 +8671,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="131" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="131" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
         <v>222</v>
       </c>
@@ -8295,7 +8687,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="132" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="132" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
         <v>224</v>
       </c>
@@ -8311,7 +8703,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="133" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="133" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
         <v>226</v>
       </c>
@@ -8327,7 +8719,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="134" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="134" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
         <v>228</v>
       </c>
@@ -8343,7 +8735,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="135" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="135" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
         <v>231</v>
       </c>
@@ -8359,7 +8751,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="136" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="136" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
         <v>234</v>
       </c>
@@ -8375,7 +8767,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="137" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="137" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
         <v>237</v>
       </c>
@@ -8391,7 +8783,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="138" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="138" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
         <v>249</v>
       </c>
@@ -8407,7 +8799,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="139" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="139" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
         <v>252</v>
       </c>
@@ -8423,7 +8815,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="140" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="140" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
         <v>255</v>
       </c>
@@ -8439,7 +8831,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="141" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="141" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
         <v>257</v>
       </c>
@@ -8455,7 +8847,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="142" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="142" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
         <v>259</v>
       </c>
@@ -8471,7 +8863,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="143" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="143" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
         <v>262</v>
       </c>
@@ -8487,7 +8879,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="144" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="144" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
         <v>265</v>
       </c>
@@ -8503,7 +8895,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="145" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="145" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
         <v>268</v>
       </c>
@@ -8519,7 +8911,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="146" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="146" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
         <v>271</v>
       </c>
@@ -8535,7 +8927,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="147" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="147" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
         <v>611</v>
       </c>
@@ -8551,7 +8943,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="148" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="148" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
         <v>274</v>
       </c>
@@ -8567,7 +8959,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="149" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="149" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
         <v>277</v>
       </c>
@@ -8583,7 +8975,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="150" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="150" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
         <v>280</v>
       </c>
@@ -8599,7 +8991,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="151" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="151" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
         <v>283</v>
       </c>
@@ -8615,7 +9007,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="152" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="152" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
         <v>616</v>
       </c>
@@ -8631,7 +9023,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="153" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="153" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A153" t="s">
         <v>297</v>
       </c>
@@ -8647,7 +9039,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="154" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="154" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
         <v>300</v>
       </c>
@@ -8663,7 +9055,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="155" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="155" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
         <v>303</v>
       </c>
@@ -8679,7 +9071,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="156" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="156" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
         <v>306</v>
       </c>
@@ -8695,7 +9087,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="157" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="157" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A157" t="s">
         <v>41</v>
       </c>
@@ -8711,7 +9103,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="158" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="158" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A158" t="s">
         <v>44</v>
       </c>
@@ -8727,7 +9119,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="159" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="159" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A159" t="s">
         <v>286</v>
       </c>
@@ -8743,7 +9135,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="160" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="160" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A160" t="s">
         <v>289</v>
       </c>
@@ -8759,7 +9151,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="161" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="161" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A161" t="s">
         <v>624</v>
       </c>
@@ -8778,7 +9170,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="162" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="162" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A162" t="s">
         <v>642</v>
       </c>
@@ -8795,7 +9187,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="163" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="163" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A163" t="s">
         <v>294</v>
       </c>
@@ -8811,7 +9203,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="164" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="164" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A164" t="s">
         <v>239</v>
       </c>
@@ -8827,7 +9219,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="165" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="165" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A165" t="s">
         <v>242</v>
       </c>
@@ -8843,7 +9235,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="166" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="166" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A166" t="s">
         <v>628</v>
       </c>
@@ -8862,7 +9254,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="167" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="167" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A167" t="s">
         <v>629</v>
       </c>
@@ -8881,7 +9273,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="168" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="168" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A168" t="s">
         <v>53</v>
       </c>
@@ -8897,7 +9289,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="169" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="169" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A169" t="s">
         <v>56</v>
       </c>
@@ -8913,9 +9305,9 @@
         <v>16</v>
       </c>
     </row>
-    <row r="170" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="170" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A170" t="s">
-        <v>656</v>
+        <v>654</v>
       </c>
       <c r="C170" t="str">
         <f t="shared" si="2"/>
@@ -8929,7 +9321,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="171" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="171" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A171" t="s">
         <v>633</v>
       </c>
@@ -8945,7 +9337,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="172" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="172" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A172" t="s">
         <v>451</v>
       </c>
@@ -8961,7 +9353,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="173" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="173" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A173" t="s">
         <v>455</v>
       </c>

</xml_diff>